<commit_message>
Elaborato 1 openmp semidefinitivo
</commit_message>
<xml_diff>
--- a/elaborati_open_mp/elaborato_1/test_valutazione_integrale.xlsx
+++ b/elaborati_open_mp/elaborato_1/test_valutazione_integrale.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fabio/Desktop/CP/GIT/Calcolo-Parallelo/elaborati_open_mp/elaborato_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D8F26CE-9EEE-5147-8107-DD62EB5EBB14}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{208AEADF-0FB2-B141-B923-8C4F46D14D7F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="7900" windowWidth="18200" windowHeight="12580" xr2:uid="{506EAF39-E1AB-4CEC-B2C8-8A63472D1D26}"/>
+    <workbookView xWindow="0" yWindow="480" windowWidth="33600" windowHeight="19940" xr2:uid="{506EAF39-E1AB-4CEC-B2C8-8A63472D1D26}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -243,24 +243,6 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -285,10 +267,28 @@
     <xf numFmtId="167" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="167" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -605,8 +605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3838E36-3F33-4BD8-8326-A9F63397C565}">
   <dimension ref="A2:M46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C2" zoomScale="125" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16:G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -651,19 +651,19 @@
       <c r="B4" s="12">
         <v>2</v>
       </c>
-      <c r="C4" s="37">
+      <c r="C4" s="31">
         <v>2.9639999993378002E-3</v>
       </c>
-      <c r="D4" s="30">
+      <c r="D4" s="24">
         <v>3.9400000023306E-3</v>
       </c>
-      <c r="E4" s="31">
+      <c r="E4" s="25">
         <v>2.04179999927874E-2</v>
       </c>
-      <c r="F4" s="29">
+      <c r="F4" s="23">
         <v>0.15014300000621</v>
       </c>
-      <c r="G4" s="32">
+      <c r="G4" s="26">
         <v>1.44200700000423</v>
       </c>
     </row>
@@ -671,19 +671,19 @@
       <c r="B5" s="12">
         <v>4</v>
       </c>
-      <c r="C5" s="37">
+      <c r="C5" s="31">
         <v>3.2320000027539E-3</v>
       </c>
-      <c r="D5" s="30">
+      <c r="D5" s="24">
         <v>4.1659999988042E-3</v>
       </c>
-      <c r="E5" s="31">
+      <c r="E5" s="25">
         <v>1.06040000027861E-2</v>
       </c>
-      <c r="F5" s="29">
+      <c r="F5" s="23">
         <v>8.0880000001343405E-2</v>
       </c>
-      <c r="G5" s="32">
+      <c r="G5" s="26">
         <v>0.72061800000083098</v>
       </c>
     </row>
@@ -691,19 +691,19 @@
       <c r="B6" s="13">
         <v>8</v>
       </c>
-      <c r="C6" s="33">
+      <c r="C6" s="27">
         <v>5.6699999986448996E-3</v>
       </c>
-      <c r="D6" s="34">
+      <c r="D6" s="28">
         <v>7.0559999971418E-3</v>
       </c>
-      <c r="E6" s="35">
+      <c r="E6" s="29">
         <v>1.17259999935632E-2</v>
       </c>
-      <c r="F6" s="33">
+      <c r="F6" s="27">
         <v>4.7178999993775499E-2</v>
       </c>
-      <c r="G6" s="36">
+      <c r="G6" s="30">
         <v>0.36798999999534998</v>
       </c>
     </row>
@@ -832,23 +832,23 @@
       <c r="B16" s="12">
         <v>2</v>
       </c>
-      <c r="C16" s="23">
+      <c r="C16" s="33">
         <f>C10/2</f>
         <v>6.8488529551890387E-2</v>
       </c>
-      <c r="D16" s="24">
+      <c r="D16" s="34">
         <f>D10/2</f>
         <v>0.4348984773169608</v>
       </c>
-      <c r="E16" s="24">
+      <c r="E16" s="34">
         <f>E10/2</f>
         <v>0.82603585109771605</v>
       </c>
-      <c r="F16" s="23">
+      <c r="F16" s="33">
         <f>F10/2</f>
         <v>0.97590963275511089</v>
       </c>
-      <c r="G16" s="25">
+      <c r="G16" s="35">
         <f>G10/2</f>
         <v>0.99332874250606162</v>
       </c>
@@ -857,23 +857,23 @@
       <c r="B17" s="12">
         <v>4</v>
       </c>
-      <c r="C17" s="23">
+      <c r="C17" s="33">
         <f>C11/4</f>
         <v>3.140470318277834E-2</v>
       </c>
-      <c r="D17" s="23">
+      <c r="D17" s="33">
         <f>D11/4</f>
         <v>0.20565290472086406</v>
       </c>
-      <c r="E17" s="23">
+      <c r="E17" s="33">
         <f>E11/4</f>
         <v>0.79526593725593731</v>
       </c>
-      <c r="F17" s="23">
+      <c r="F17" s="33">
         <f>F11/4</f>
         <v>0.9058234421017386</v>
       </c>
-      <c r="G17" s="26">
+      <c r="G17" s="36">
         <f>G11/4</f>
         <v>0.99386013116345162</v>
       </c>
@@ -882,23 +882,23 @@
       <c r="B18" s="13">
         <v>8</v>
       </c>
-      <c r="C18" s="27">
+      <c r="C18" s="37">
         <f>C12/8</f>
         <v>8.9506173542753947E-3</v>
       </c>
-      <c r="D18" s="27">
+      <c r="D18" s="37">
         <f>D12/8</f>
         <v>6.0710742713169417E-2</v>
       </c>
-      <c r="E18" s="27">
+      <c r="E18" s="37">
         <f>E12/8</f>
         <v>0.35958553664961668</v>
       </c>
-      <c r="F18" s="27">
+      <c r="F18" s="37">
         <f>F12/8</f>
         <v>0.77643655024556868</v>
       </c>
-      <c r="G18" s="28">
+      <c r="G18" s="38">
         <f>G12/8</f>
         <v>0.97311543793122102</v>
       </c>
@@ -948,7 +948,7 @@
       <c r="F22" s="5">
         <v>0.29305199999362203</v>
       </c>
-      <c r="G22" s="38">
+      <c r="G22" s="32">
         <v>2.8647739999982802</v>
       </c>
     </row>

</xml_diff>